<commit_message>
Actualizar mi logt y task
</commit_message>
<xml_diff>
--- a/tspi/ciclo-2/logt1/20105914.xlsx
+++ b/tspi/ciclo-2/logt1/20105914.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Preparacion para presentacion de Rails</t>
+  </si>
+  <si>
+    <t>Presentar al equipo herramienta Rails</t>
   </si>
 </sst>
 </file>
@@ -183,18 +186,6 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -227,6 +218,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,243 +562,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK12"/>
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="3" width="10.83203125" style="6"/>
-    <col min="4" max="4" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="7"/>
-    <col min="6" max="7" width="10.83203125" style="8"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
-    <col min="9" max="1025" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="6" max="7" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="10.83203125" style="5"/>
+    <col min="9" max="1025" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="16"/>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="17">
         <v>41923</v>
       </c>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="13">
-      <c r="A2" s="10" t="s">
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="18"/>
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="13">
-      <c r="A3" s="10" t="s">
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="19">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="13">
-      <c r="E5" s="7">
+      <c r="G3" s="19"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="E5" s="3">
         <f>SUM(E7:E12)/60</f>
         <v>9.5833333333333339</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="52">
-      <c r="A7" s="5">
+      <c r="A7" s="1">
         <v>41924</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>0.63541666666666696</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="2">
         <v>0.65625</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="7">
-        <f>((HOUR(C7)-HOUR(B7))*60)+(MINUTE(C7)-MINUTE(B7))-D7</f>
+      <c r="E7" s="3">
+        <f t="shared" ref="E7:E13" si="0">((HOUR(C7)-HOUR(B7))*60)+(MINUTE(C7)-MINUTE(B7))-D7</f>
         <v>30</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <v>24</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="65">
-      <c r="A8" s="5">
+      <c r="A8" s="1">
         <v>41924</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>0.65972222222222199</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="2">
         <v>0.67708333333333304</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="E8" s="7">
-        <f>((HOUR(C8)-HOUR(B8))*60)+(MINUTE(C8)-MINUTE(B8))-D8</f>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="13">
         <v>25</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="39">
-      <c r="A9" s="5">
+      <c r="A9" s="1">
         <v>41926</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>0.39791666666666697</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="2">
         <v>0.41319444444444398</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="7">
-        <f>((HOUR(C9)-HOUR(B9))*60)+(MINUTE(C9)-MINUTE(B9))-D9</f>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="13">
         <v>30</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="52">
-      <c r="A10" s="5">
+      <c r="A10" s="1">
         <v>41926</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="2">
         <v>0.98263888888888884</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="7">
-        <f>((HOUR(C10)-HOUR(B10))*60)+(MINUTE(C10)-MINUTE(B10))-D10</f>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
         <v>195</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="13">
         <v>31</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="52">
-      <c r="A11" s="5">
+      <c r="A11" s="1">
         <v>41928</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="2">
         <v>0.375</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="3">
         <v>35</v>
       </c>
-      <c r="E11" s="7">
-        <f>((HOUR(C11)-HOUR(B11))*60)+(MINUTE(C11)-MINUTE(B11))-D11</f>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
         <v>265</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="13">
         <v>42</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="52">
-      <c r="A12" s="5">
+      <c r="A12" s="1">
         <v>41931</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="2">
         <v>0.68333333333333302</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="2">
         <v>0.70972222222222203</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="3">
         <v>0</v>
       </c>
-      <c r="E12" s="7">
-        <f>((HOUR(C12)-HOUR(B12))*60)+(MINUTE(C12)-MINUTE(B12))-D12</f>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="13">
         <v>32</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="15" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="52">
+      <c r="A13" s="1">
+        <v>41931</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F13" s="4">
+        <v>43</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>